<commit_message>
Updated Test Case excel
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,32 +1,259 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25906"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imsam\Desktop\Ngee Ann Poly Work\Year 3\Sem 2\DevOps\DevOps_Oct2022_Team5_Week3\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{15695338-D211-4A47-A30F-42F4F213BE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FBCFD49-45CB-4AE3-AB4E-7F15F636F783}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+  <si>
+    <t>Test Case ID</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Prerequsites</t>
+  </si>
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Can automate</t>
+  </si>
+  <si>
+    <t>Search function loading speed</t>
+  </si>
+  <si>
+    <t>Testing loading speed of searching a book in search form</t>
+  </si>
+  <si>
+    <t>1. Select search text box
+2. Type "C# for dummies"
+3. Click Go
+4. Wait 10 seconds</t>
+  </si>
+  <si>
+    <t>Test Fail loading speed more than 10 sec</t>
+  </si>
+  <si>
+    <t>Find Library location</t>
+  </si>
+  <si>
+    <t>Change default library location &amp; find the location of selected library</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Change library to Sengkang Public Library
+2. Click "Go to the library"
+3. See page change </t>
+  </si>
+  <si>
+    <t>Test passes, page display's location of Sengkang Public Library</t>
+  </si>
+  <si>
+    <t>Subscribe to eNewsletter</t>
+  </si>
+  <si>
+    <t>Subcribe to NLB's eNewsletter to receive emails and eNewsletters</t>
+  </si>
+  <si>
+    <t>1. Select Subscribe Now
+2. Enter email into the Forum
+3. Click Submit Now button</t>
+  </si>
+  <si>
+    <t>Chatbox/Chatbot</t>
+  </si>
+  <si>
+    <t>Rate website</t>
+  </si>
+  <si>
+    <t>Give a 2 star rating on the website</t>
+  </si>
+  <si>
+    <t>1. Click on rating
+2. select 2 smiley faces
+3. Type "This is a test"
+4. Enter personnel email in email box
+5. Click submit</t>
+  </si>
+  <si>
+    <t>Test pass, it reads thank you for your feedback</t>
+  </si>
+  <si>
+    <t>Filtering facility type for bookings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">filter facility type for booking of rooms </t>
+  </si>
+  <si>
+    <t>1. Click on book room or revenue
+2. Click on the drop down of facility type
+3. Choose meeting room filter</t>
+  </si>
+  <si>
+    <t>All the facilities that is for meeting room will be shown</t>
+  </si>
+  <si>
+    <t>Loan eBook(s)</t>
+  </si>
+  <si>
+    <t>Borrow eBooks through NLB's website</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">1. Select </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Loans and Reservations
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">2. Click </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">Borrow eBooks
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>3. Enter Login Details</t>
+    </r>
+  </si>
+  <si>
+    <t>Redirecting to social media links</t>
+  </si>
+  <si>
+    <t>Check if the redirection of social media link is working</t>
+  </si>
+  <si>
+    <t>1. Click on the instagram icon, facebook icon, linkedin icon, youtube icon, twitter icon
+2. redirected to a new page</t>
+  </si>
+  <si>
+    <t>based on what icon you have clicked it will redirect you to the specific page</t>
+  </si>
+  <si>
+    <t>Search book name</t>
+  </si>
+  <si>
+    <t>Enter a book name and view results</t>
+  </si>
+  <si>
+    <t>1. Select search text box
+2. Type "C# for dummies"
+3. Click Go</t>
+  </si>
+  <si>
+    <t>Test succeeds, results display all books similar to "C# for dummies"</t>
+  </si>
+  <si>
+    <t>Feedback form validation</t>
+  </si>
+  <si>
+    <t>Test the validation of feedback form from nlb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on contact us
+2. Click on hyperlink "online"
+3. redirected to feedback form page
+4. try entering email 123
+5. try entering letters in contact
+6. try leaving suggestion and name empty
+</t>
+  </si>
+  <si>
+    <t>Please enter valid email error message appears, letters are not being inputted into the contact fieldbox, when submit button is pressed this field is required appears on both suggestion and name fieldbox</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +276,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +563,476 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="19.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="91.5">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="91.5">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="91.5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" ht="121.5">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="91.5">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="76.5">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="121.5">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="76.5">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" ht="198">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004F6724D69C4A2643B32EC3B349496B98" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="327c39f43b88a996ce8b5f7a4b7e5bdf">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a5a90c7d-0e98-467f-9b04-54754a86672d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c0c1e1c7d4482a9fb7b60639323fb3b1" ns2:_="">
+    <xsd:import namespace="a5a90c7d-0e98-467f-9b04-54754a86672d"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a5a90c7d-0e98-467f-9b04-54754a86672d" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C5D14E-D1D0-4EBA-AB65-3DD8F8AFF9EB}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51922A53-A7DB-4A96-AA60-0A6C84577C07}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7970275B-6D47-442C-8D5A-F4AFF2227D5E}"/>
 </file>
</xml_diff>

<commit_message>
Update TestCases excel file
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imsam\Desktop\Ngee Ann Poly Work\Year 3\Sem 2\DevOps\DevOps_Oct2022_Team5_Week3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectnpedu.sharepoint.com/sites/NamelessTeam/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="13_ncr:1_{15695338-D211-4A47-A30F-42F4F213BE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FBCFD49-45CB-4AE3-AB4E-7F15F636F783}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{15695338-D211-4A47-A30F-42F4F213BE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4371CB8F-1669-4A30-99D4-C5FE78966432}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Can automate</t>
+  </si>
+  <si>
+    <t>Elgin</t>
   </si>
   <si>
     <t>Search function loading speed</t>
@@ -100,9 +103,6 @@
     <t>1. Select Subscribe Now
 2. Enter email into the Forum
 3. Click Submit Now button</t>
-  </si>
-  <si>
-    <t>Chatbox/Chatbot</t>
   </si>
   <si>
     <t>Rate website</t>
@@ -231,12 +231,158 @@
   <si>
     <t>Please enter valid email error message appears, letters are not being inputted into the contact fieldbox, when submit button is pressed this field is required appears on both suggestion and name fieldbox</t>
   </si>
+  <si>
+    <t>Submit Feedback</t>
+  </si>
+  <si>
+    <t>Submit a Feedback Form</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Tricia</t>
+  </si>
+  <si>
+    <t>Jun Jie</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Contact Us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Click on the Hyperlink "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Online</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"
+3. Redirect to Feedback Form Page
+4. Fill in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Comments/Suggestions </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Text Box
+5. Fill in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> text box
+6. Fill in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> text box
+7. Submit Feedback Form
+8. On Thanks page, click 5 star rating
+9. Type "Great" into Feedback experience box
+10. Submit Feedback Experience Form</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Pass, Popup will appear with text "Thank you for submitting your feedback!"</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Yes?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,6 +400,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -299,6 +453,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,317 +722,343 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="19.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="91.5">
-      <c r="A2">
+    <row r="2" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="91.5">
-      <c r="A3">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
         <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="1"/>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="91.5">
-      <c r="A4">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
         <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>44</v>
+      </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="121.5">
-      <c r="A6">
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="91.5">
-      <c r="A7">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="76.5">
-      <c r="A8">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="1"/>
+      <c r="F8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="121.5">
-      <c r="A9">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="76.5">
-      <c r="A10">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="198">
-      <c r="A11">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12">
         <v>11</v>
       </c>
-      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13">
         <v>12</v>
       </c>
-      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="B14" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="B15" s="1"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="B16" s="1"/>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="1"/>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="1"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1026,13 +1210,43 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C5D14E-D1D0-4EBA-AB65-3DD8F8AFF9EB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C5D14E-D1D0-4EBA-AB65-3DD8F8AFF9EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a5a90c7d-0e98-467f-9b04-54754a86672d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51922A53-A7DB-4A96-AA60-0A6C84577C07}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{51922A53-A7DB-4A96-AA60-0A6C84577C07}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a5a90c7d-0e98-467f-9b04-54754a86672d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7970275B-6D47-442C-8D5A-F4AFF2227D5E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7970275B-6D47-442C-8D5A-F4AFF2227D5E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Kevin's test case, updated excel file
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://connectnpedu.sharepoint.com/sites/NamelessTeam/Shared Documents/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\DevOps\DevOps_Oct2022_Team5_Week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="13_ncr:1_{15695338-D211-4A47-A30F-42F4F213BE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4371CB8F-1669-4A30-99D4-C5FE78966432}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E24287-1F59-4C52-8C95-A15B6E267675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="61">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -59,7 +59,7 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>Can automate</t>
+    <t>Testable</t>
   </si>
   <si>
     <t>Elgin</t>
@@ -80,6 +80,9 @@
     <t>Test Fail loading speed more than 10 sec</t>
   </si>
   <si>
+    <t>Kevin</t>
+  </si>
+  <si>
     <t>Find Library location</t>
   </si>
   <si>
@@ -94,6 +97,9 @@
     <t>Test passes, page display's location of Sengkang Public Library</t>
   </si>
   <si>
+    <t>Tricia</t>
+  </si>
+  <si>
     <t>Subscribe to eNewsletter</t>
   </si>
   <si>
@@ -103,6 +109,146 @@
     <t>1. Select Subscribe Now
 2. Enter email into the Forum
 3. Click Submit Now button</t>
+  </si>
+  <si>
+    <t>Test passes, Successfully subscribes to the newsletter</t>
+  </si>
+  <si>
+    <t>Jun Jie</t>
+  </si>
+  <si>
+    <t>Submit Feedback</t>
+  </si>
+  <si>
+    <t>Submit a Feedback Form</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Contact Us</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Click on the Hyperlink "</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Online</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"
+3. Redirect to Feedback Form Page
+4. Fill in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Comments/Suggestions </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Text Box
+5. Fill in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> text box
+6. Fill in </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Email</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> text box
+7. Submit Feedback Form
+8. On Thanks page, click 5 star rating
+9. Type "Great" into Feedback experience box
+10. Submit Feedback Experience Form</t>
+    </r>
+  </si>
+  <si>
+    <t>Test Pass, Popup will appear with text "Thank you for submitting your feedback!"</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Samuel</t>
   </si>
   <si>
     <t>Rate website</t>
@@ -146,6 +292,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">1. Select </t>
     </r>
@@ -155,6 +302,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Loans and Reservations
 </t>
@@ -164,6 +312,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">2. Click </t>
     </r>
@@ -173,6 +322,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Borrow eBooks
 </t>
@@ -182,6 +332,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>3. Enter Login Details</t>
     </r>
@@ -232,150 +383,32 @@
     <t>Please enter valid email error message appears, letters are not being inputted into the contact fieldbox, when submit button is pressed this field is required appears on both suggestion and name fieldbox</t>
   </si>
   <si>
-    <t>Submit Feedback</t>
-  </si>
-  <si>
-    <t>Submit a Feedback Form</t>
-  </si>
-  <si>
-    <t>Kevin</t>
-  </si>
-  <si>
-    <t>Tricia</t>
-  </si>
-  <si>
-    <t>Jun Jie</t>
-  </si>
-  <si>
-    <t>Samuel</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Contact Us</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2. Click on the Hyperlink "</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Online</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"
-3. Redirect to Feedback Form Page
-4. Fill in </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Comments/Suggestions </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Text Box
-5. Fill in </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Name</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> text box
-6. Fill in </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Email</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> text box
-7. Submit Feedback Form
-8. On Thanks page, click 5 star rating
-9. Type "Great" into Feedback experience box
-10. Submit Feedback Experience Form</t>
-    </r>
-  </si>
-  <si>
-    <t>Test Pass, Popup will appear with text "Thank you for submitting your feedback!"</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Yes?</t>
+    <t>Confirm Registration
+with Singpass</t>
+  </si>
+  <si>
+    <t>Test if the registration works for singpass</t>
+  </si>
+  <si>
+    <t>1. Click on the person icon at the top right of the website.
+2. Click on Apply now!
+3. Use Singpass 
+4. Create an account with singpass</t>
+  </si>
+  <si>
+    <t>Registration successful</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Page efficiency</t>
+  </si>
+  <si>
+    <t>Testing the efficiency to drill down from main page all the way down</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -394,12 +427,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -453,10 +488,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,20 +755,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="120" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="19.26953125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +795,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -784,225 +816,249 @@
         <v>12</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+      <c r="I2" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="I4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I13" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1011,7 +1067,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1020,7 +1076,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1029,7 +1085,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1038,7 +1094,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1047,7 +1103,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1212,15 +1268,8 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C5D14E-D1D0-4EBA-AB65-3DD8F8AFF9EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a5a90c7d-0e98-467f-9b04-54754a86672d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added screenshot of test cases passing
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imsam\Desktop\Ngee Ann Poly Work\Year 3\Sem 2\DevOps\DevOps_Oct2022_Team5_Week3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Documents\DevOps\DevOps_Oct2022_Team5_Week3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A06EBB1-7BBB-4D17-82E7-95CDF2674370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D60C253A-3293-4B78-88D6-2D66A8B7D90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,6 +488,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>163224</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1210304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3453FD3-9E86-3418-1C81-FB8A28C7D8B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8896350" y="184150"/>
+          <a:ext cx="9307224" cy="4505954"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -757,19 +806,19 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="6" max="7" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -795,7 +844,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -822,7 +871,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -849,7 +898,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -876,7 +925,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="360" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="302.39999999999998" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -903,7 +952,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="100.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>5</v>
       </c>
@@ -923,7 +972,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>6</v>
       </c>
@@ -943,7 +992,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>7</v>
       </c>
@@ -961,7 +1010,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -988,7 +1037,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>9</v>
       </c>
@@ -1008,7 +1057,7 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>10</v>
       </c>
@@ -1028,7 +1077,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>11</v>
       </c>
@@ -1049,7 +1098,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>12</v>
       </c>
@@ -1066,7 +1115,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1075,7 +1124,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1084,7 +1133,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1093,7 +1142,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1102,7 +1151,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1111,7 +1160,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1123,16 +1172,14 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1268,15 +1315,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7970275B-6D47-442C-8D5A-F4AFF2227D5E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C5D14E-D1D0-4EBA-AB65-3DD8F8AFF9EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1300,10 +1351,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13C5D14E-D1D0-4EBA-AB65-3DD8F8AFF9EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7970275B-6D47-442C-8D5A-F4AFF2227D5E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>